<commit_message>
journal entry method refactored
</commit_message>
<xml_diff>
--- a/PLCashbook/TestDocuments/PLC_Test Scenarios.xlsx
+++ b/PLCashbook/TestDocuments/PLC_Test Scenarios.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
   <si>
     <t>Completed</t>
   </si>
@@ -627,7 +627,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -687,7 +689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="120">
+    <row r="3" spans="1:7" ht="102.75" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -806,7 +808,9 @@
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="2"/>

</xml_diff>